<commit_message>
Author        : Priyanka Chaudhary Description   : Updated Plan for NSKFDC App File Updated  : WorkPlan-Updated.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-Updated.xlsx
+++ b/Requirements/WorkPlan-Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC BUG FIXING\NSKFDC\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{85211CE5-038E-4429-90A4-E1E175861E7D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ACD11055-4878-4CD6-9FEC-1670675284D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="1" xr2:uid="{BCF9E9A8-2EA7-413C-AB62-EB238F3EA7A6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{BCF9E9A8-2EA7-413C-AB62-EB238F3EA7A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Priyanka" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
   <si>
     <t>Issue ID</t>
   </si>
@@ -386,7 +386,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,12 +492,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -668,7 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -680,8 +673,8 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,12 +687,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75015335-51C3-445C-9F44-9BF8A8A26570}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,10 +1124,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="30"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="55" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="1"/>
@@ -1159,13 +1152,11 @@
         <v>2.25</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="56" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="55" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="1"/>
@@ -1190,9 +1181,9 @@
         <v>1.5</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="J4" s="33" t="s">
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="J4" s="32" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="1"/>
@@ -1218,10 +1209,9 @@
         <v>1.5</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="33" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="33" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="1"/>
@@ -1246,12 +1236,12 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="32" t="s">
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="33" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="1"/>
@@ -1278,12 +1268,11 @@
         <v>3</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="32" t="s">
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="J7" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1307,8 +1296,8 @@
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1336,8 +1325,8 @@
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1365,8 +1354,8 @@
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1394,8 +1383,8 @@
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1423,8 +1412,8 @@
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1452,8 +1441,8 @@
         <v>0</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1481,8 +1470,8 @@
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1505,8 +1494,8 @@
       <c r="F15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="1" t="s">
         <v>92</v>
       </c>
@@ -1541,8 +1530,8 @@
       <c r="F16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="7" t="s">
         <v>85</v>
       </c>
@@ -1558,30 +1547,30 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="55">
+      <c r="B17" s="52"/>
+      <c r="C17" s="54">
         <f>SUM(C2:C14)</f>
         <v>27</v>
       </c>
-      <c r="D17" s="55">
+      <c r="D17" s="54">
         <f>SUM(D2:D14)</f>
         <v>8.25</v>
       </c>
-      <c r="E17" s="55">
+      <c r="E17" s="54">
         <f>SUM(E2:E14)</f>
         <v>18.75</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
-      <c r="P17" s="55"/>
+      <c r="P17" s="54"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1599,8 +1588,8 @@
         <v>3</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1621,10 +1610,10 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="52">
+      <c r="C23" s="51">
         <v>19</v>
       </c>
     </row>
@@ -1650,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4405F3-3AA3-44FA-8F3F-D711A4F518C3}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,23 +1719,23 @@
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="42"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="1">
         <f>(C2-D2)</f>
         <v>3</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="44" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1759,23 +1748,23 @@
       <c r="C3" s="2">
         <v>1.5</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="1">
         <f>(C3-D3)</f>
         <v>1.5</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="44" t="s">
         <v>43</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1788,23 +1777,23 @@
       <c r="C4" s="2">
         <v>1.5</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="1">
         <f>(C4-D4)</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1817,54 +1806,54 @@
       <c r="C5" s="29">
         <v>7.5</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="1">
         <f>(C5-D5)</f>
         <v>7.5</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="34" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="33" t="s">
         <v>54</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="37">
         <v>0.75</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="1">
         <f>(C6-D6)</f>
         <v>0.75</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1877,7 +1866,7 @@
       <c r="C7" s="2">
         <v>2.5</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="40">
         <v>2.5</v>
       </c>
       <c r="E7" s="1">
@@ -1885,15 +1874,15 @@
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1906,7 +1895,7 @@
       <c r="C8" s="2">
         <v>0.75</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="40">
         <v>0.75</v>
       </c>
       <c r="E8" s="1">
@@ -1914,15 +1903,15 @@
         <v>0</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1935,7 +1924,7 @@
       <c r="C9" s="2">
         <v>0.75</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="40">
         <v>0.75</v>
       </c>
       <c r="E9" s="1">
@@ -1943,15 +1932,15 @@
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1964,7 +1953,7 @@
       <c r="C10" s="2">
         <v>1.5</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="40">
         <v>1.5</v>
       </c>
       <c r="E10" s="1">
@@ -1972,15 +1961,15 @@
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1993,7 +1982,7 @@
       <c r="C11" s="2">
         <v>0.75</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="40">
         <v>0.75</v>
       </c>
       <c r="E11" s="1">
@@ -2001,15 +1990,15 @@
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2022,7 +2011,7 @@
       <c r="C12" s="2">
         <v>0.75</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="40">
         <v>0.75</v>
       </c>
       <c r="E12" s="1">
@@ -2030,15 +2019,15 @@
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2051,7 +2040,7 @@
       <c r="C13" s="2">
         <v>4.5</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="42">
         <v>4.5</v>
       </c>
       <c r="E13" s="1">
@@ -2059,15 +2048,15 @@
         <v>0</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2080,7 +2069,7 @@
       <c r="C14" s="2">
         <v>0.75</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <v>0.75</v>
       </c>
       <c r="E14" s="1">
@@ -2088,15 +2077,15 @@
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2112,8 +2101,8 @@
       <c r="F15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="7" t="s">
         <v>85</v>
       </c>
@@ -2129,30 +2118,30 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54">
+      <c r="B16" s="52"/>
+      <c r="C16" s="53">
         <f>SUM(C2:C14)</f>
         <v>26.5</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="53">
         <f>SUM(D7:D14)</f>
         <v>12.25</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="54">
         <f t="shared" si="0"/>
         <v>14.25</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="55"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="54"/>
     </row>
     <row r="17" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -2164,7 +2153,7 @@
       <c r="C17" s="2">
         <v>2</v>
       </c>
-      <c r="D17" s="42"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="1">
         <f>(C17-D17)</f>
         <v>2</v>
@@ -2172,15 +2161,15 @@
       <c r="F17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
       <c r="P17" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2202,10 +2191,10 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="52">
+      <c r="C22" s="51">
         <v>15</v>
       </c>
     </row>
@@ -2264,19 +2253,19 @@
       <c r="H1" s="4">
         <v>29</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="48" t="s">
         <v>72</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="49" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="3">
@@ -2304,26 +2293,26 @@
         <f t="shared" ref="E2:E10" si="0">(C2-D2)</f>
         <v>15</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="34" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>59</v>
       </c>
       <c r="L2" s="32" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2341,18 +2330,18 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2370,18 +2359,18 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2402,15 +2391,15 @@
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2431,15 +2420,15 @@
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2460,15 +2449,15 @@
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2484,8 +2473,8 @@
       <c r="F8" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="7" t="s">
         <v>85</v>
       </c>
@@ -2501,30 +2490,30 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46">
+      <c r="B9" s="45"/>
+      <c r="C9" s="45">
         <f>SUM(C2:C7)</f>
         <v>23.5</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="45">
         <f>SUM(D2:D7)</f>
         <v>7.5</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="45">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="46"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="45"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2542,20 +2531,20 @@
         <v>6</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="34" t="s">
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="33" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2568,10 +2557,10 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="51">
         <v>16</v>
       </c>
     </row>
@@ -2647,7 +2636,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="50" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author        : Priyanka Chaudhary Description   : Updated Gantt Chart - Pooja File Updated  : WorkPlan-Updated.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/WorkPlan-Updated.xlsx
+++ b/Requirements/WorkPlan-Updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC BUG FIXING\NSKFDC\trunk\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ACD11055-4878-4CD6-9FEC-1670675284D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CD65950D-CBB7-4FB2-B2D0-21273EFE867C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" xr2:uid="{BCF9E9A8-2EA7-413C-AB62-EB238F3EA7A6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="1" xr2:uid="{BCF9E9A8-2EA7-413C-AB62-EB238F3EA7A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Priyanka" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="97">
   <si>
     <t>Issue ID</t>
   </si>
@@ -195,9 +195,6 @@
     <t>NA-2</t>
   </si>
   <si>
-    <t>Upload Documents - Training Partner | 7.5 Hrs</t>
-  </si>
-  <si>
     <t>NA-86</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Deploy NSKFDC App on AWS | 3hr</t>
+  </si>
+  <si>
+    <t>Upload Documents - Training Partner | 11.5 Hrs</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -654,11 +654,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -672,7 +670,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,6 +690,15 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75015335-51C3-445C-9F44-9BF8A8A26570}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,16 +1072,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="G1" s="4">
         <v>28</v>
@@ -1084,19 +1090,19 @@
         <v>29</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>75</v>
       </c>
       <c r="N1" s="3">
         <v>4</v>
@@ -1105,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1123,17 +1129,17 @@
         <f>(C2-D2)</f>
         <v>2</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="52" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1152,17 +1158,17 @@
         <v>2.25</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="52" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1181,16 +1187,16 @@
         <v>1.5</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="J4" s="32" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="J4" s="30" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1209,16 +1215,16 @@
         <v>1.5</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="33" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="31" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1236,20 +1242,20 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="33" t="s">
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1268,24 +1274,24 @@
         <v>3</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="J7" s="32" t="s">
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="J7" s="30" t="s">
         <v>24</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -1296,15 +1302,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1325,15 +1331,15 @@
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1354,15 +1360,15 @@
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1383,15 +1389,15 @@
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1412,15 +1418,15 @@
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1441,15 +1447,15 @@
         <v>0</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1470,107 +1476,107 @@
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="22"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+        <v>91</v>
+      </c>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
+        <v>91</v>
+      </c>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
       <c r="P15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="22"/>
       <c r="E16" s="1"/>
       <c r="F16" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
+        <v>84</v>
+      </c>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="54">
+      <c r="B17" s="49"/>
+      <c r="C17" s="51">
         <f>SUM(C2:C14)</f>
         <v>27</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="51">
         <f>SUM(D2:D14)</f>
         <v>8.25</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="51">
         <f>SUM(E2:E14)</f>
         <v>18.75</v>
       </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="54"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="51"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1588,32 +1594,32 @@
         <v>3</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="32" t="s">
+      <c r="M18" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
       <c r="P18" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="23">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="51">
+      <c r="B23" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="48">
         <v>19</v>
       </c>
     </row>
@@ -1623,10 +1629,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1639,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4405F3-3AA3-44FA-8F3F-D711A4F518C3}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,16 +1673,16 @@
         <v>28</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="G1" s="3">
         <v>28</v>
@@ -1685,19 +1691,19 @@
         <v>29</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>75</v>
       </c>
       <c r="N1" s="3">
         <v>4</v>
@@ -1706,7 +1712,7 @@
         <v>5</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1719,23 +1725,23 @@
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="1">
         <f>(C2-D2)</f>
         <v>3</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="41" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1748,23 +1754,23 @@
       <c r="C3" s="2">
         <v>1.5</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="1">
         <f>(C3-D3)</f>
         <v>1.5</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="41" t="s">
         <v>43</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1777,83 +1783,86 @@
       <c r="C4" s="2">
         <v>1.5</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="1">
         <f>(C4-D4)</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="29">
-        <v>7.5</v>
-      </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="1">
-        <f>(C5-D5)</f>
-        <v>7.5</v>
-      </c>
-      <c r="F5" s="34" t="s">
+      <c r="B5" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="56">
+        <v>11.5</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="53">
+        <v>11.5</v>
+      </c>
+      <c r="F5" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="33" t="s">
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>54</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="37">
+      <c r="B6" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="35">
         <v>0.75</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="1">
         <f>(C6-D6)</f>
         <v>0.75</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
+      <c r="F6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1866,7 +1875,7 @@
       <c r="C7" s="2">
         <v>2.5</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="38">
         <v>2.5</v>
       </c>
       <c r="E7" s="1">
@@ -1874,15 +1883,15 @@
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1895,7 +1904,7 @@
       <c r="C8" s="2">
         <v>0.75</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="38">
         <v>0.75</v>
       </c>
       <c r="E8" s="1">
@@ -1903,15 +1912,15 @@
         <v>0</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1924,7 +1933,7 @@
       <c r="C9" s="2">
         <v>0.75</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="38">
         <v>0.75</v>
       </c>
       <c r="E9" s="1">
@@ -1932,15 +1941,15 @@
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1953,7 +1962,7 @@
       <c r="C10" s="2">
         <v>1.5</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="38">
         <v>1.5</v>
       </c>
       <c r="E10" s="1">
@@ -1961,15 +1970,15 @@
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1982,7 +1991,7 @@
       <c r="C11" s="2">
         <v>0.75</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="38">
         <v>0.75</v>
       </c>
       <c r="E11" s="1">
@@ -1990,15 +1999,15 @@
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2011,7 +2020,7 @@
       <c r="C12" s="2">
         <v>0.75</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="38">
         <v>0.75</v>
       </c>
       <c r="E12" s="1">
@@ -2019,15 +2028,15 @@
         <v>0</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2040,7 +2049,7 @@
       <c r="C13" s="2">
         <v>4.5</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="40">
         <v>4.5</v>
       </c>
       <c r="E13" s="1">
@@ -2048,15 +2057,15 @@
         <v>0</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2069,7 +2078,7 @@
       <c r="C14" s="2">
         <v>0.75</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="38">
         <v>0.75</v>
       </c>
       <c r="E14" s="1">
@@ -2077,73 +2086,73 @@
         <v>0</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="22"/>
       <c r="E15" s="1"/>
       <c r="F15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+        <v>84</v>
+      </c>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53">
+      <c r="B16" s="49"/>
+      <c r="C16" s="50">
         <f>SUM(C2:C14)</f>
-        <v>26.5</v>
-      </c>
-      <c r="D16" s="53">
+        <v>30.5</v>
+      </c>
+      <c r="D16" s="50">
         <f>SUM(D7:D14)</f>
         <v>12.25</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="51">
         <f t="shared" si="0"/>
-        <v>14.25</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="54"/>
-    </row>
-    <row r="17" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+        <v>18.25</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="51"/>
+    </row>
+    <row r="17" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
@@ -2153,48 +2162,48 @@
       <c r="C17" s="2">
         <v>2</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="1">
         <f>(C17-D17)</f>
         <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+        <v>87</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K19" s="28"/>
+      <c r="K19" s="27"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
-      <c r="B20" s="26"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="27"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="23">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="51">
+      <c r="B22" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="48">
         <v>15</v>
       </c>
     </row>
@@ -2236,16 +2245,16 @@
         <v>53</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="G1" s="4">
         <v>28</v>
@@ -2253,20 +2262,20 @@
       <c r="H1" s="4">
         <v>29</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="K1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="M1" s="46" t="s">
         <v>74</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>75</v>
       </c>
       <c r="N1" s="3">
         <v>4</v>
@@ -2275,15 +2284,15 @@
         <v>5</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="C2" s="1">
         <v>15</v>
@@ -2293,34 +2302,34 @@
         <f t="shared" ref="E2:E10" si="0">(C2-D2)</f>
         <v>15</v>
       </c>
-      <c r="F2" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>59</v>
+      <c r="F2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1">
         <v>0.5</v>
@@ -2330,26 +2339,26 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="F3" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1">
         <v>0.5</v>
@@ -2359,18 +2368,18 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="F4" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2378,7 +2387,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1">
         <v>2.5</v>
@@ -2391,23 +2400,23 @@
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -2420,23 +2429,23 @@
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -2449,78 +2458,78 @@
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="22"/>
       <c r="E8" s="1"/>
       <c r="F8" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+        <v>84</v>
+      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42">
         <f>SUM(C2:C7)</f>
         <v>23.5</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="42">
         <f>SUM(D2:D7)</f>
         <v>7.5</v>
       </c>
-      <c r="E9" s="45">
+      <c r="E9" s="42">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="45"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="42"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
@@ -2531,36 +2540,36 @@
         <v>6</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="M10" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="33" t="s">
-        <v>56</v>
+      <c r="L10" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="23">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="51">
+      <c r="B17" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="48">
         <v>16</v>
       </c>
     </row>
@@ -2588,22 +2597,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>75</v>
       </c>
       <c r="H1" s="3">
         <v>4</v>
@@ -2612,15 +2621,15 @@
         <v>5</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -2630,14 +2639,14 @@
         <f>(C2-D2)</f>
         <v>3</v>
       </c>
-      <c r="F2" s="32" t="s">
-        <v>67</v>
+      <c r="F2" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="50" t="s">
-        <v>67</v>
+      <c r="J2" s="47" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>